<commit_message>
Upodated with issue tracker
</commit_message>
<xml_diff>
--- a/CAV Schedules/AHU 1_CAV.xlsx
+++ b/CAV Schedules/AHU 1_CAV.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rushikesh/Documents/PsychroCalc/CAV Schedules/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rush\OneDrive - SC Engineers\Documents\Desktop\PsychroCalc\CAV Schedules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9522AAA-882F-E64A-92C7-076E80FC1D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C4BB778-EF74-4C89-A467-86FFE7663748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="2300" windowWidth="27640" windowHeight="16940" xr2:uid="{C5DF299C-43A3-0D48-8AAA-BA2E3FFCC1AB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C6828FA9-C442-49A1-9452-1356960703C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -112,7 +112,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -563,24 +563,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B271B635-F2EC-7A46-8A2B-59938835D076}" name="AHU 1Table4A" displayName="AHU_1Table4A" ref="A1:O40" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:O40" xr:uid="{B271B635-F2EC-7A46-8A2B-59938835D076}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BEE8C5C1-4029-44E3-8932-FF7A9877B042}" name="AHU 1Table4A" displayName="AHU_1Table4A" ref="A1:O40" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A1:O40" xr:uid="{BEE8C5C1-4029-44E3-8932-FF7A9877B042}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{F9779D0B-7DE4-C64A-B29A-F100FC91B3D5}" name="BASIS OF DESIGN _x000a_MANUFACTURER" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{8D017F8E-35A2-264B-BBED-82F7856C75D2}" name="DESCRIPTION" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{574FB132-F03B-2742-809D-0ABD78A53685}" name="CFM" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{EF99993D-09B3-E44D-BFBD-C895807FB21F}" name="CAV INLET SIZE" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{2F5BD8E0-799C-AF4F-B69F-C3F05257E486}" name="MAX TOTAL CAV PD _x000a_(IN W.G.)" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{B39FF64F-BADC-8442-B2DC-64AB9AF317E5}" name="EWT" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{EEEE42CE-77DC-A744-A76B-B329FDD59401}" name="DESIGN _x000a_LWT" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{4C71A4F7-4718-564B-AF26-D1EE1A92D21F}" name="EAT" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{A64E150E-300D-B541-B706-9D22FFDBD380}" name="DESIGN _x000a_LAT" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{BA7E6F71-126F-3E41-89F0-5E6586D4EDBA}" name="AGPM" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{26531501-C5F3-984E-AC16-389C2941CE34}" name="GPM" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{E966E52C-C9EF-5746-9B74-53A7CE1F015C}" name="MAX WATER _x000a_PD (FT)" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{03ACE895-13EB-EA4A-8829-6C5F4388AE4B}" name="OPER _x000a_WEIGHT_x000a_(LBS)" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{4C90AE09-EAF0-2442-8976-1E0D9FE63C85}" name="MTG _x000a_DETAIL" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{BA93EF8D-89EF-EB44-957A-AAB69FD40DB7}" name="REMARKS" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{DA799785-9F88-416F-AE9F-E3E7F34E75DC}" name="BASIS OF DESIGN _x000a_MANUFACTURER" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{40B200CA-4E21-4E47-9F81-AA8D95E72EEB}" name="DESCRIPTION" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{83C154F2-B605-41FF-845F-EC0B7D58A550}" name="CFM" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{A4472AC1-D18F-4452-9463-F9BEFBD0895A}" name="CAV INLET SIZE" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{AD41C136-ABD5-4A21-9655-3192D4F67115}" name="MAX TOTAL CAV PD _x000a_(IN W.G.)" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{012B5B27-D1AC-468A-BE15-628F28BC49D3}" name="EWT" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{DC93309A-BAD3-4FB0-A7F7-77890B32C0B7}" name="DESIGN _x000a_LWT" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{D1E68D5D-ED55-40C3-813D-EC74D1516CBE}" name="EAT" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{C268388E-533F-453C-B80F-0764757C78A7}" name="DESIGN _x000a_LAT" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{39499F6B-3C5B-470B-B547-0C32B18D7F69}" name="AGPM" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{FD9434D0-F42B-4CA2-A75F-D00C00C426AB}" name="GPM" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{4D8DD5AB-58D0-41F0-8BC2-B5DE51759178}" name="MAX WATER _x000a_PD (FT)" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{EF794A05-DCC7-4640-8D3D-EA4275CC0759}" name="OPER _x000a_WEIGHT_x000a_(LBS)" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{B94E6104-7C8C-4063-8D93-FF888B84043A}" name="MTG _x000a_DETAIL" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{6F3E9F9B-79A4-41A0-B73C-050E2952B232}" name="REMARKS" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -882,33 +882,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FDC3239-35C1-214C-AA93-B7936B097BBF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9434FC7-81EB-43A7-B90E-BC319D5E4CBD}">
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J1" sqref="J1:R40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -955,7 +955,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>9</v>
       </c>
@@ -2130,7 +2130,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>9</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>9</v>
       </c>
@@ -2224,7 +2224,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>9</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>9</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>9</v>
       </c>
@@ -2412,7 +2412,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>9</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>9</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>9</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>9</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>9</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>9</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>

</xml_diff>